<commit_message>
simplified version without powo names and gbif
</commit_message>
<xml_diff>
--- a/docs/occ_fields_translator.xlsx
+++ b/docs/occ_fields_translator.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\geocat_staging\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\sb42kg\geocat_staging\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{412C96D2-E77C-45B0-A760-62F76DE57302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDC6258-58B6-43E3-B776-73DD283CE765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="24510" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SRLI_2_points_template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="248">
   <si>
     <t>COMBINED</t>
   </si>
@@ -181,9 +194,6 @@
     <t>IUCN points field - see mapping standards</t>
   </si>
   <si>
-    <t>binomial</t>
-  </si>
-  <si>
     <t>DETBY</t>
   </si>
   <si>
@@ -761,6 +771,12 @@
   </si>
   <si>
     <t>specificEpithet</t>
+  </si>
+  <si>
+    <t>sci_name</t>
+  </si>
+  <si>
+    <t>yrcompiled</t>
   </si>
 </sst>
 </file>
@@ -1256,11 +1272,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1622,7 +1636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,7 +1645,7 @@
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
@@ -1641,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1649,7 +1663,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1668,7 +1682,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -1676,7 +1690,7 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
@@ -1694,13 +1708,13 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>53</v>
+      <c r="E3" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -1711,7 +1725,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1719,7 +1733,7 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
@@ -1734,16 +1748,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>219</v>
+      <c r="E5" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1754,7 +1768,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1762,7 +1776,7 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
@@ -1771,42 +1785,42 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
         <v>151</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
         <v>153</v>
       </c>
-      <c r="F7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>154</v>
-      </c>
-      <c r="H7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -1814,106 +1828,106 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" t="s">
         <v>85</v>
       </c>
-      <c r="B9" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
         <v>87</v>
-      </c>
-      <c r="H9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
         <v>137</v>
       </c>
-      <c r="B10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" t="s">
         <v>139</v>
       </c>
-      <c r="F10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>140</v>
-      </c>
-      <c r="H10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" t="s">
         <v>142</v>
       </c>
-      <c r="B11" t="s">
-        <v>241</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
         <v>144</v>
       </c>
-      <c r="F11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>145</v>
-      </c>
-      <c r="H11" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" t="s">
         <v>93</v>
       </c>
-      <c r="B12" t="s">
-        <v>241</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>94</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" t="s">
         <v>97</v>
-      </c>
-      <c r="H12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1921,12 +1935,12 @@
         <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F13" t="s">
@@ -1935,218 +1949,218 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
         <v>112</v>
       </c>
-      <c r="B14" t="s">
-        <v>240</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" t="s">
         <v>114</v>
-      </c>
-      <c r="F14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
         <v>192</v>
       </c>
-      <c r="B15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" t="s">
         <v>193</v>
       </c>
-      <c r="D15" t="s">
-        <v>192</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" t="s">
         <v>194</v>
       </c>
-      <c r="F15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>195</v>
-      </c>
-      <c r="H15" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" t="s">
         <v>187</v>
       </c>
-      <c r="B16" t="s">
-        <v>241</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
         <v>189</v>
       </c>
-      <c r="F16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>190</v>
-      </c>
-      <c r="H16" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" t="s">
         <v>89</v>
       </c>
-      <c r="B17" t="s">
-        <v>241</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" t="s">
         <v>91</v>
-      </c>
-      <c r="H17" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>172</v>
+      <c r="E18" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
       </c>
       <c r="G18" t="s">
+        <v>172</v>
+      </c>
+      <c r="H18" t="s">
         <v>173</v>
-      </c>
-      <c r="H18" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>176</v>
+      <c r="E19" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
       </c>
       <c r="G19" t="s">
+        <v>176</v>
+      </c>
+      <c r="H19" t="s">
         <v>177</v>
-      </c>
-      <c r="H19" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" t="s">
         <v>69</v>
       </c>
-      <c r="B20" t="s">
-        <v>240</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
       </c>
       <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
         <v>72</v>
-      </c>
-      <c r="H20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
-        <v>241</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="F21" t="s">
         <v>14</v>
       </c>
       <c r="G21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" t="s">
         <v>81</v>
-      </c>
-      <c r="H21" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>180</v>
+      <c r="E22" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
@@ -2154,16 +2168,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" t="s">
         <v>184</v>
       </c>
-      <c r="B23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E23" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -2171,62 +2185,62 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" t="s">
         <v>229</v>
       </c>
-      <c r="B24" t="s">
-        <v>240</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E24" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>231</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24" t="s">
+        <v>231</v>
+      </c>
+      <c r="H24" t="s">
         <v>232</v>
-      </c>
-      <c r="H24" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" t="s">
+        <v>239</v>
+      </c>
+      <c r="C25" t="s">
         <v>164</v>
       </c>
-      <c r="B25" t="s">
-        <v>240</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E25" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" t="s">
         <v>166</v>
       </c>
-      <c r="F25" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>167</v>
-      </c>
-      <c r="H25" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C26" t="s">
-        <v>220</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>97</v>
+        <v>219</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
@@ -2237,7 +2251,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -2260,7 +2274,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -2283,7 +2297,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" t="s">
         <v>32</v>
@@ -2295,7 +2309,7 @@
         <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H29" t="s">
         <v>33</v>
@@ -2306,7 +2320,7 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
@@ -2329,7 +2343,7 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -2346,7 +2360,7 @@
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -2369,7 +2383,7 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C33" t="s">
         <v>45</v>
@@ -2386,128 +2400,128 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" t="s">
-        <v>240</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
         <v>55</v>
       </c>
-      <c r="D34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>56</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>57</v>
-      </c>
-      <c r="H34" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" t="s">
         <v>59</v>
       </c>
-      <c r="B35" t="s">
-        <v>241</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" t="s">
         <v>60</v>
       </c>
-      <c r="D35" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>61</v>
-      </c>
-      <c r="H35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" t="s">
         <v>63</v>
       </c>
-      <c r="B36" t="s">
-        <v>241</v>
-      </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H36" t="s">
         <v>61</v>
-      </c>
-      <c r="H36" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37" t="s">
         <v>65</v>
       </c>
-      <c r="B37" t="s">
-        <v>241</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
-      </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" t="s">
         <v>61</v>
-      </c>
-      <c r="H37" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" t="s">
         <v>67</v>
       </c>
-      <c r="B38" t="s">
-        <v>240</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
-      </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" t="s">
         <v>61</v>
-      </c>
-      <c r="H38" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
-        <v>240</v>
-      </c>
-      <c r="C39" t="s">
-        <v>75</v>
-      </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -2515,16 +2529,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>239</v>
+      </c>
+      <c r="C40" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
-        <v>240</v>
-      </c>
-      <c r="C40" t="s">
-        <v>77</v>
-      </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F40" t="s">
         <v>14</v>
@@ -2532,16 +2546,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="s">
-        <v>240</v>
-      </c>
-      <c r="C41" t="s">
-        <v>84</v>
-      </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -2549,16 +2563,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" t="s">
         <v>99</v>
       </c>
-      <c r="B42" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" t="s">
-        <v>100</v>
-      </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -2566,338 +2580,338 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
+        <v>239</v>
+      </c>
+      <c r="C43" t="s">
         <v>101</v>
       </c>
-      <c r="B43" t="s">
-        <v>240</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" t="s">
         <v>102</v>
       </c>
-      <c r="D43" t="s">
-        <v>101</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>103</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>104</v>
-      </c>
-      <c r="H43" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" t="s">
         <v>106</v>
       </c>
-      <c r="B44" t="s">
-        <v>240</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" t="s">
         <v>107</v>
       </c>
-      <c r="D44" t="s">
-        <v>106</v>
-      </c>
-      <c r="F44" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>108</v>
-      </c>
-      <c r="H44" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" t="s">
         <v>110</v>
       </c>
-      <c r="B45" t="s">
-        <v>240</v>
-      </c>
-      <c r="C45" t="s">
-        <v>111</v>
-      </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G45" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" t="s">
         <v>108</v>
-      </c>
-      <c r="H45" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>239</v>
+      </c>
+      <c r="C46" t="s">
         <v>116</v>
       </c>
-      <c r="B46" t="s">
-        <v>240</v>
-      </c>
-      <c r="C46" t="s">
-        <v>117</v>
-      </c>
       <c r="D46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" t="s">
+        <v>239</v>
+      </c>
+      <c r="C47" t="s">
         <v>118</v>
       </c>
-      <c r="B47" t="s">
-        <v>240</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>119</v>
       </c>
-      <c r="D47" t="s">
-        <v>120</v>
-      </c>
       <c r="F47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" t="s">
+        <v>241</v>
+      </c>
+      <c r="C48" t="s">
         <v>121</v>
       </c>
-      <c r="B48" t="s">
-        <v>242</v>
-      </c>
-      <c r="C48" t="s">
-        <v>122</v>
-      </c>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" t="s">
+        <v>241</v>
+      </c>
+      <c r="C49" t="s">
         <v>123</v>
       </c>
-      <c r="B49" t="s">
-        <v>242</v>
-      </c>
-      <c r="C49" t="s">
-        <v>124</v>
-      </c>
       <c r="D49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" t="s">
+        <v>241</v>
+      </c>
+      <c r="C50" t="s">
         <v>125</v>
       </c>
-      <c r="B50" t="s">
-        <v>242</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
-      </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" t="s">
         <v>127</v>
       </c>
-      <c r="B51" t="s">
-        <v>240</v>
-      </c>
-      <c r="C51" t="s">
-        <v>128</v>
-      </c>
       <c r="D51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" t="s">
         <v>129</v>
       </c>
-      <c r="B52" t="s">
-        <v>242</v>
-      </c>
-      <c r="C52" t="s">
-        <v>130</v>
-      </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" t="s">
+        <v>241</v>
+      </c>
+      <c r="C53" t="s">
         <v>131</v>
       </c>
-      <c r="B53" t="s">
-        <v>242</v>
-      </c>
-      <c r="C53" t="s">
-        <v>132</v>
-      </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" t="s">
         <v>133</v>
       </c>
-      <c r="B54" t="s">
-        <v>242</v>
-      </c>
-      <c r="C54" t="s">
-        <v>134</v>
-      </c>
       <c r="D54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" t="s">
         <v>135</v>
       </c>
-      <c r="B55" t="s">
-        <v>240</v>
-      </c>
-      <c r="C55" t="s">
-        <v>136</v>
-      </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
+        <v>239</v>
+      </c>
+      <c r="C56" t="s">
         <v>147</v>
       </c>
-      <c r="B56" t="s">
-        <v>240</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" t="s">
         <v>148</v>
       </c>
-      <c r="D56" t="s">
-        <v>147</v>
-      </c>
-      <c r="F56" t="s">
-        <v>103</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>149</v>
-      </c>
-      <c r="H56" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" t="s">
         <v>156</v>
       </c>
-      <c r="B57" t="s">
-        <v>240</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>155</v>
+      </c>
+      <c r="F57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G57" t="s">
         <v>157</v>
       </c>
-      <c r="D57" t="s">
-        <v>156</v>
-      </c>
-      <c r="F57" t="s">
-        <v>103</v>
-      </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>158</v>
-      </c>
-      <c r="H57" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>159</v>
+      </c>
+      <c r="B58" t="s">
+        <v>239</v>
+      </c>
+      <c r="C58" t="s">
         <v>160</v>
       </c>
-      <c r="B58" t="s">
-        <v>240</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="F58" t="s">
+        <v>102</v>
+      </c>
+      <c r="G58" t="s">
         <v>161</v>
       </c>
-      <c r="F58" t="s">
-        <v>103</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>162</v>
-      </c>
-      <c r="H58" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" t="s">
+        <v>239</v>
+      </c>
+      <c r="C59" t="s">
         <v>169</v>
       </c>
-      <c r="B59" t="s">
-        <v>240</v>
-      </c>
-      <c r="C59" t="s">
-        <v>170</v>
-      </c>
       <c r="D59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>196</v>
+      </c>
+      <c r="B60" t="s">
+        <v>239</v>
+      </c>
+      <c r="C60" t="s">
         <v>197</v>
       </c>
-      <c r="B60" t="s">
-        <v>240</v>
-      </c>
-      <c r="C60" t="s">
-        <v>198</v>
-      </c>
       <c r="D60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F60" t="s">
         <v>14</v>
@@ -2905,16 +2919,16 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B61" t="s">
+        <v>239</v>
+      </c>
+      <c r="C61" t="s">
         <v>199</v>
       </c>
-      <c r="B61" t="s">
-        <v>240</v>
-      </c>
-      <c r="C61" t="s">
-        <v>200</v>
-      </c>
       <c r="D61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F61" t="s">
         <v>14</v>
@@ -2922,16 +2936,16 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>200</v>
+      </c>
+      <c r="B62" t="s">
+        <v>239</v>
+      </c>
+      <c r="C62" t="s">
         <v>201</v>
       </c>
-      <c r="B62" t="s">
-        <v>240</v>
-      </c>
-      <c r="C62" t="s">
-        <v>202</v>
-      </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F62" t="s">
         <v>14</v>
@@ -2939,39 +2953,39 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" t="s">
+        <v>239</v>
+      </c>
+      <c r="C63" t="s">
         <v>203</v>
       </c>
-      <c r="B63" t="s">
-        <v>240</v>
-      </c>
-      <c r="C63" t="s">
-        <v>204</v>
-      </c>
       <c r="D63" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" t="s">
         <v>14</v>
       </c>
       <c r="G63" t="s">
+        <v>204</v>
+      </c>
+      <c r="H63" t="s">
         <v>205</v>
-      </c>
-      <c r="H63" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" t="s">
+        <v>239</v>
+      </c>
+      <c r="C64" t="s">
         <v>207</v>
       </c>
-      <c r="B64" t="s">
-        <v>240</v>
-      </c>
-      <c r="C64" t="s">
-        <v>208</v>
-      </c>
       <c r="D64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F64" t="s">
         <v>14</v>
@@ -2979,16 +2993,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" t="s">
+        <v>239</v>
+      </c>
+      <c r="C65" t="s">
         <v>209</v>
       </c>
-      <c r="B65" t="s">
-        <v>240</v>
-      </c>
-      <c r="C65" t="s">
-        <v>210</v>
-      </c>
       <c r="D65" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
@@ -2996,16 +3010,16 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66" t="s">
+        <v>239</v>
+      </c>
+      <c r="C66" t="s">
         <v>211</v>
       </c>
-      <c r="B66" t="s">
-        <v>240</v>
-      </c>
-      <c r="C66" t="s">
-        <v>212</v>
-      </c>
       <c r="D66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -3013,16 +3027,16 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" t="s">
+        <v>239</v>
+      </c>
+      <c r="C67" t="s">
         <v>213</v>
       </c>
-      <c r="B67" t="s">
-        <v>240</v>
-      </c>
-      <c r="C67" t="s">
-        <v>214</v>
-      </c>
       <c r="D67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F67" t="s">
         <v>14</v>
@@ -3030,16 +3044,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>214</v>
+      </c>
+      <c r="B68" t="s">
+        <v>239</v>
+      </c>
+      <c r="C68" t="s">
         <v>215</v>
       </c>
-      <c r="B68" t="s">
-        <v>240</v>
-      </c>
-      <c r="C68" t="s">
-        <v>216</v>
-      </c>
       <c r="D68" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F68" t="s">
         <v>14</v>
@@ -3047,16 +3061,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B69" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F69" t="s">
         <v>14</v>
@@ -3064,16 +3078,16 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" t="s">
+        <v>239</v>
+      </c>
+      <c r="C70" t="s">
         <v>221</v>
       </c>
-      <c r="B70" t="s">
-        <v>240</v>
-      </c>
-      <c r="C70" t="s">
-        <v>222</v>
-      </c>
       <c r="D70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F70" t="s">
         <v>24</v>
@@ -3081,16 +3095,16 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>222</v>
+      </c>
+      <c r="B71" t="s">
+        <v>239</v>
+      </c>
+      <c r="C71" t="s">
         <v>223</v>
       </c>
-      <c r="B71" t="s">
-        <v>240</v>
-      </c>
-      <c r="C71" t="s">
-        <v>224</v>
-      </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F71" t="s">
         <v>24</v>
@@ -3098,56 +3112,56 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>224</v>
+      </c>
+      <c r="B72" t="s">
+        <v>239</v>
+      </c>
+      <c r="C72" t="s">
         <v>225</v>
       </c>
-      <c r="B72" t="s">
-        <v>240</v>
-      </c>
-      <c r="C72" t="s">
-        <v>226</v>
-      </c>
       <c r="D72" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F72" t="s">
         <v>24</v>
       </c>
       <c r="G72" t="s">
+        <v>226</v>
+      </c>
+      <c r="H72" t="s">
         <v>227</v>
-      </c>
-      <c r="H72" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" t="s">
+        <v>239</v>
+      </c>
+      <c r="C73" t="s">
         <v>234</v>
       </c>
-      <c r="B73" t="s">
-        <v>240</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="F73" t="s">
         <v>235</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>236</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>237</v>
-      </c>
-      <c r="H73" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>243</v>
+      </c>
+      <c r="B74" t="s">
+        <v>239</v>
+      </c>
+      <c r="C74" t="s">
         <v>244</v>
-      </c>
-      <c r="B74" t="s">
-        <v>240</v>
-      </c>
-      <c r="C74" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>